<commit_message>
send mail to me every day
</commit_message>
<xml_diff>
--- a/Docs/report_alpha.xlsx
+++ b/Docs/report_alpha.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="53">
   <si>
     <t>EURUSD</t>
   </si>
@@ -204,15 +204,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>万点</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2w</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1w</t>
+    <t>sugg_new</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -702,9 +694,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:V30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F7" sqref="F7"/>
+      <selection pane="bottomLeft" activeCell="F1" sqref="F1:M1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -714,14 +706,14 @@
     <col min="3" max="3" width="8.75" style="1" customWidth="1"/>
     <col min="4" max="4" width="8.125" style="1" customWidth="1"/>
     <col min="5" max="5" width="7.625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="9.25" style="4" customWidth="1"/>
-    <col min="7" max="7" width="7.875" style="4" customWidth="1"/>
-    <col min="8" max="8" width="12.125" style="4" customWidth="1"/>
-    <col min="9" max="9" width="7.875" style="4" customWidth="1"/>
-    <col min="10" max="10" width="9.375" style="3" customWidth="1"/>
-    <col min="11" max="11" width="9" style="3" customWidth="1"/>
-    <col min="12" max="12" width="8" style="3" customWidth="1"/>
-    <col min="13" max="13" width="8.25" style="3" customWidth="1"/>
+    <col min="6" max="6" width="9.25" style="4" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="7.875" style="4" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="12.125" style="4" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="7.875" style="4" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="9.375" style="3" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="9" style="3" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="8" style="3" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="8.25" style="3" hidden="1" customWidth="1"/>
     <col min="14" max="17" width="9" style="2" customWidth="1"/>
     <col min="18" max="19" width="9" style="2"/>
     <col min="20" max="20" width="12.5" style="2" customWidth="1"/>
@@ -846,13 +838,13 @@
         <v>39</v>
       </c>
       <c r="Q2" s="15">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="R2" s="15" t="s">
         <v>36</v>
       </c>
       <c r="S2" s="15">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="T2" s="15">
         <v>0.01</v>
@@ -861,7 +853,7 @@
         <v>622</v>
       </c>
       <c r="V2" s="15">
-        <v>1.2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:22" s="19" customFormat="1">
@@ -970,7 +962,7 @@
         <v>655</v>
       </c>
       <c r="V4" s="17">
-        <v>1.2</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="5" spans="1:22">
@@ -1116,7 +1108,7 @@
       <c r="H7" s="18">
         <v>0.43</v>
       </c>
-      <c r="I7" s="18">
+      <c r="I7" s="22">
         <v>0.24</v>
       </c>
       <c r="J7" s="17">
@@ -1147,7 +1139,7 @@
         <v>36</v>
       </c>
       <c r="S7" s="17">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="T7" s="17">
         <v>0.01</v>
@@ -1156,7 +1148,7 @@
         <v>442</v>
       </c>
       <c r="V7" s="17">
-        <v>0.8</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="9" spans="1:22">
@@ -1345,7 +1337,7 @@
       <c r="H13" s="18">
         <v>0.38</v>
       </c>
-      <c r="I13" s="18">
+      <c r="I13" s="22">
         <v>0.24</v>
       </c>
       <c r="J13" s="17">
@@ -1385,7 +1377,7 @@
         <v>603</v>
       </c>
       <c r="V13" s="17">
-        <v>1</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="15" spans="1:22" s="23" customFormat="1">
@@ -1719,8 +1711,8 @@
       <c r="U22" s="21">
         <v>1779</v>
       </c>
-      <c r="V22" s="21" t="s">
-        <v>53</v>
+      <c r="V22" s="21">
+        <v>0.02</v>
       </c>
     </row>
     <row r="24" spans="1:22" s="17" customFormat="1">
@@ -1787,8 +1779,8 @@
       <c r="U24" s="17">
         <v>500</v>
       </c>
-      <c r="V24" s="17" t="s">
-        <v>54</v>
+      <c r="V24" s="17">
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:22" s="19" customFormat="1">

</xml_diff>